<commit_message>
Make corrections following R, RStudio update
</commit_message>
<xml_diff>
--- a/PFNA_Unit_Conversion_v2_kwon_options.xlsx
+++ b/PFNA_Unit_Conversion_v2_kwon_options.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24931"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/larsen_alexandra_epa_gov/Documents/Projects/IRIS/PFAS/pfas-birthweight-meta-analysis/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_99AFB14D8385C1DB1449BD8C4353BF42988B8B57" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{64C110E7-6548-49B6-A4E3-1B5FD41CE0D9}"/>
   <bookViews>
-    <workbookView/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PFNA" sheetId="1" r:id="rId1"/>
@@ -304,9 +310,6 @@
     <t>Wikstrom 2020</t>
   </si>
   <si>
-    <t>Wikström, 2020</t>
-  </si>
-  <si>
     <t>Chen 2021 1st</t>
   </si>
   <si>
@@ -350,12 +353,15 @@
   </si>
   <si>
     <t>Wang, 2016 Girl</t>
+  </si>
+  <si>
+    <t>Wikstrom, 2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="10">
     <numFmt numFmtId="164" formatCode="##0.00"/>
     <numFmt numFmtId="165" formatCode="###############0"/>
@@ -368,7 +374,7 @@
     <numFmt numFmtId="172" formatCode="###0.0"/>
     <numFmt numFmtId="173" formatCode="#0.000000000"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="9.5"/>
       <color rgb="FF000000"/>
@@ -459,34 +465,34 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="172" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="173" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="173" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -495,6 +501,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -564,19 +578,19 @@
         </a:solidFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln cmpd="sng" algn="ctr" w="9525" cap="flat">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln cmpd="sng" algn="ctr" w="25400" cap="flat">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln cmpd="sng" algn="ctr" w="38100" cap="flat">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -613,51 +627,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="0" enableFormatConditionsCalculation="0">
-    <pageSetUpPr fitToPage="0"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE29"/>
   <sheetViews>
-    <sheetView zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W22" sqref="W22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="12" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.71" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.71" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.71" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.71" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.71" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.71" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.71" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.71" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.71" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.71" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.71" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.71" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.71" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.71" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.71" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.71" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.71" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.71" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.71" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.71" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.71" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.71" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.71" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.71" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.71" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.71" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.71" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.71" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.71" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.71" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.71" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="31" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14" customHeight="1">
+    <row r="1" spans="1:31" ht="13.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -752,7 +759,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" ht="14" customHeight="1">
+    <row r="2" spans="1:31" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
@@ -790,16 +797,16 @@
         <v>77.5</v>
       </c>
       <c r="M2" s="3">
-        <v>-0.2231435513142</v>
+        <v>-0.22314355131419999</v>
       </c>
       <c r="N2" s="3">
-        <v>0.37867560164257</v>
+        <v>0.37867560164257003</v>
       </c>
       <c r="O2" s="3">
         <v>27.5</v>
       </c>
       <c r="P2" s="3">
-        <v>25.5106728462327</v>
+        <v>25.510672846232701</v>
       </c>
       <c r="Q2" s="3">
         <v>-22.5</v>
@@ -808,7 +815,7 @@
         <v>77.5</v>
       </c>
       <c r="S2" s="3">
-        <v>22.1952666817841</v>
+        <v>22.195266681784101</v>
       </c>
       <c r="T2" s="3">
         <v>20.5896795292321</v>
@@ -817,7 +824,7 @@
         <v>-18.159763648732</v>
       </c>
       <c r="V2" s="3">
-        <v>62.5502970123006</v>
+        <v>62.550297012300597</v>
       </c>
       <c r="W2" s="2" t="s">
         <v>34</v>
@@ -832,7 +839,7 @@
         <v>36</v>
       </c>
       <c r="AA2" s="7">
-        <v>11.624</v>
+        <v>11.624000000000001</v>
       </c>
       <c r="AB2" s="2" t="s">
         <v>37</v>
@@ -847,15 +854,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" ht="14" customHeight="1">
+    <row r="3" spans="1:31" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B3" s="3">
-        <v>0.763</v>
+        <v>0.76300000000000001</v>
       </c>
       <c r="C3" s="3">
-        <v>0.531</v>
+        <v>0.53100000000000003</v>
       </c>
       <c r="D3" s="3">
         <v>1.155</v>
@@ -876,43 +883,43 @@
         <v>40</v>
       </c>
       <c r="J3" s="3">
-        <v>0.51296556192979</v>
+        <v>0.51296556192979004</v>
       </c>
       <c r="K3" s="3">
-        <v>-82.429619913179</v>
+        <v>-82.429619913178996</v>
       </c>
       <c r="L3" s="3">
-        <v>83.455551037039</v>
+        <v>83.455551037039001</v>
       </c>
       <c r="M3" s="3">
-        <v>-0.2704972476977</v>
+        <v>-0.27049724769770001</v>
       </c>
       <c r="N3" s="3">
-        <v>0.57606034911128</v>
+        <v>0.57606034911128001</v>
       </c>
       <c r="O3" s="3">
-        <v>0.28386821828014</v>
+        <v>0.28386821828013997</v>
       </c>
       <c r="P3" s="3">
         <v>23.4184442450304</v>
       </c>
       <c r="Q3" s="3">
-        <v>-45.615439075939</v>
+        <v>-45.615439075939001</v>
       </c>
       <c r="R3" s="3">
-        <v>46.183175512499</v>
+        <v>46.183175512498998</v>
       </c>
       <c r="S3" s="3">
-        <v>0.22234577207498</v>
+        <v>0.22234577207497999</v>
       </c>
       <c r="T3" s="3">
-        <v>18.342990624324</v>
+        <v>18.342990624323999</v>
       </c>
       <c r="U3" s="3">
-        <v>-35.729255220356</v>
+        <v>-35.729255220356002</v>
       </c>
       <c r="V3" s="3">
-        <v>36.1739467645059</v>
+        <v>36.173946764505899</v>
       </c>
       <c r="W3" s="2" t="s">
         <v>41</v>
@@ -942,7 +949,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" ht="14" customHeight="1">
+    <row r="4" spans="1:31" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>43</v>
       </c>
@@ -980,34 +987,34 @@
         <v>17.61</v>
       </c>
       <c r="M4" s="3">
-        <v>-0.5457430738374</v>
+        <v>-0.54574307383739995</v>
       </c>
       <c r="N4" s="3">
-        <v>0.51034817502521</v>
+        <v>0.51034817502521002</v>
       </c>
       <c r="O4" s="3">
-        <v>-24.901117286501</v>
+        <v>-24.901117286501002</v>
       </c>
       <c r="P4" s="3">
-        <v>34.4838045818297</v>
+        <v>34.483804581829702</v>
       </c>
       <c r="Q4" s="3">
-        <v>-92.476009085409</v>
+        <v>-92.476009085409004</v>
       </c>
       <c r="R4" s="3">
-        <v>42.6980209751981</v>
+        <v>42.698020975198098</v>
       </c>
       <c r="S4" s="3">
         <v>-14.81647806993</v>
       </c>
       <c r="T4" s="3">
-        <v>20.5182975717879</v>
+        <v>20.518297571787901</v>
       </c>
       <c r="U4" s="3">
-        <v>-55.024388859505</v>
+        <v>-55.024388859505002</v>
       </c>
       <c r="V4" s="3">
-        <v>25.4058596700547</v>
+        <v>25.405859670054699</v>
       </c>
       <c r="W4" s="2" t="s">
         <v>47</v>
@@ -1037,7 +1044,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" ht="14" customHeight="1">
+    <row r="5" spans="1:31" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>49</v>
       </c>
@@ -1060,7 +1067,7 @@
         <v>-52</v>
       </c>
       <c r="H5" s="3">
-        <v>-4.4</v>
+        <v>-4.4000000000000004</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>33</v>
@@ -1072,37 +1079,37 @@
         <v>-104</v>
       </c>
       <c r="L5" s="3">
-        <v>-8.8</v>
+        <v>-8.8000000000000007</v>
       </c>
       <c r="M5" s="3">
-        <v>-0.3566749439387</v>
+        <v>-0.35667494393869997</v>
       </c>
       <c r="N5" s="3">
-        <v>0.51383077397392</v>
+        <v>0.51383077397391996</v>
       </c>
       <c r="O5" s="3">
         <v>-56.4</v>
       </c>
       <c r="P5" s="3">
-        <v>24.2861605496135</v>
+        <v>24.286160549613498</v>
       </c>
       <c r="Q5" s="11">
         <v>-104</v>
       </c>
       <c r="R5" s="3">
-        <v>-8.8</v>
+        <v>-8.8000000000000007</v>
       </c>
       <c r="S5" s="3">
-        <v>-40.126846717792</v>
+        <v>-40.126846717791999</v>
       </c>
       <c r="T5" s="3">
-        <v>17.2788482577665</v>
+        <v>17.278848257766501</v>
       </c>
       <c r="U5" s="3">
-        <v>-73.992766997347</v>
+        <v>-73.992766997347005</v>
       </c>
       <c r="V5" s="3">
-        <v>-6.2609264382371</v>
+        <v>-6.2609264382371004</v>
       </c>
       <c r="W5" s="2" t="s">
         <v>50</v>
@@ -1132,7 +1139,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" ht="14" customHeight="1">
+    <row r="6" spans="1:31" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>51</v>
       </c>
@@ -1143,7 +1150,7 @@
         <v>0.7</v>
       </c>
       <c r="D6" s="3">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>52</v>
@@ -1155,7 +1162,7 @@
         <v>-159.49</v>
       </c>
       <c r="H6" s="3">
-        <v>143.48</v>
+        <v>143.47999999999999</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>53</v>
@@ -1167,37 +1174,37 @@
         <v>-159.49</v>
       </c>
       <c r="L6" s="3">
-        <v>143.48</v>
+        <v>143.47999999999999</v>
       </c>
       <c r="M6" s="3">
         <v>-0.1053605156578</v>
       </c>
       <c r="N6" s="3">
-        <v>0.51372084219091</v>
+        <v>0.51372084219090997</v>
       </c>
       <c r="O6" s="3">
         <v>-8</v>
       </c>
       <c r="P6" s="3">
-        <v>77.2896855222312</v>
+        <v>77.289685522231196</v>
       </c>
       <c r="Q6" s="11">
         <v>-159.49</v>
       </c>
       <c r="R6" s="3">
-        <v>143.48</v>
+        <v>143.47999999999999</v>
       </c>
       <c r="S6" s="3">
-        <v>-7.3179152125606</v>
+        <v>-7.3179152125606004</v>
       </c>
       <c r="T6" s="3">
-        <v>70.6999206821448</v>
+        <v>70.699920682144807</v>
       </c>
       <c r="U6" s="11">
         <v>-145.89178715641</v>
       </c>
       <c r="V6" s="3">
-        <v>131.246809337274</v>
+        <v>131.24680933727399</v>
       </c>
       <c r="W6" s="2" t="s">
         <v>54</v>
@@ -1212,7 +1219,7 @@
         <v>36</v>
       </c>
       <c r="AA6" s="10">
-        <v>18.1</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="AB6" s="2" t="s">
         <v>55</v>
@@ -1227,7 +1234,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" ht="14" customHeight="1">
+    <row r="7" spans="1:31" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>57</v>
       </c>
@@ -1265,16 +1272,16 @@
         <v>-11.2</v>
       </c>
       <c r="M7" s="3">
-        <v>-0.9162907318742</v>
+        <v>-0.91629073187419996</v>
       </c>
       <c r="N7" s="3">
-        <v>0.51383077397392</v>
+        <v>0.51383077397391996</v>
       </c>
       <c r="O7" s="11">
-        <v>-140.17356940762</v>
+        <v>-140.17356940761999</v>
       </c>
       <c r="P7" s="3">
-        <v>57.6741597884789</v>
+        <v>57.674159788478903</v>
       </c>
       <c r="Q7" s="11">
         <v>-253.33452387731</v>
@@ -1286,7 +1293,7 @@
         <v>-57.6</v>
       </c>
       <c r="T7" s="3">
-        <v>23.6994150741502</v>
+        <v>23.699415074150199</v>
       </c>
       <c r="U7" s="11">
         <v>-104.1</v>
@@ -1322,7 +1329,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" ht="14" customHeight="1">
+    <row r="8" spans="1:31" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>61</v>
       </c>
@@ -1360,34 +1367,34 @@
         <v>25</v>
       </c>
       <c r="M8" s="3">
-        <v>-0.5276327420824</v>
+        <v>-0.52763274208239996</v>
       </c>
       <c r="N8" s="3">
-        <v>0.40090042582406</v>
+        <v>0.40090042582405999</v>
       </c>
       <c r="O8" s="11">
-        <v>-101.02612498362</v>
+        <v>-101.02612498361999</v>
       </c>
       <c r="P8" s="3">
-        <v>81.6127400736891</v>
+        <v>81.612740073689096</v>
       </c>
       <c r="Q8" s="11">
-        <v>-259.78146424359</v>
+        <v>-259.78146424358999</v>
       </c>
       <c r="R8" s="3">
-        <v>60.1345982045336</v>
+        <v>60.134598204533603</v>
       </c>
       <c r="S8" s="3">
-        <v>-60.593191717336</v>
+        <v>-60.593191717335998</v>
       </c>
       <c r="T8" s="3">
-        <v>48.9494812026508</v>
+        <v>48.949481202650801</v>
       </c>
       <c r="U8" s="11">
         <v>-155.81106441601</v>
       </c>
       <c r="V8" s="3">
-        <v>36.0673760222241</v>
+        <v>36.067376022224103</v>
       </c>
       <c r="W8" s="2" t="s">
         <v>62</v>
@@ -1417,7 +1424,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" ht="14" customHeight="1">
+    <row r="9" spans="1:31" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>64</v>
       </c>
@@ -1437,7 +1444,7 @@
         <v>6.07</v>
       </c>
       <c r="G9" s="3">
-        <v>-16.6</v>
+        <v>-16.600000000000001</v>
       </c>
       <c r="H9" s="3">
         <v>28.7</v>
@@ -1449,28 +1456,28 @@
         <v>6.07</v>
       </c>
       <c r="K9" s="3">
-        <v>-16.6</v>
+        <v>-16.600000000000001</v>
       </c>
       <c r="L9" s="3">
         <v>28.7</v>
       </c>
       <c r="M9" s="3">
-        <v>0.85866161903752</v>
+        <v>0.85866161903752003</v>
       </c>
       <c r="N9" s="3">
         <v>1.55603713570699</v>
       </c>
       <c r="O9" s="3">
-        <v>2.03327692989219</v>
+        <v>2.0332769298921902</v>
       </c>
       <c r="P9" s="3">
-        <v>3.87104265924468</v>
+        <v>3.8710426592446798</v>
       </c>
       <c r="Q9" s="3">
-        <v>-5.5605266945981</v>
+        <v>-5.5605266945981002</v>
       </c>
       <c r="R9" s="3">
-        <v>9.6136816948774</v>
+        <v>9.6136816948773998</v>
       </c>
       <c r="S9" s="3">
         <v>6.07</v>
@@ -1479,7 +1486,7 @@
         <v>11.5563347993434</v>
       </c>
       <c r="U9" s="3">
-        <v>-16.6</v>
+        <v>-16.600000000000001</v>
       </c>
       <c r="V9" s="3">
         <v>28.7</v>
@@ -1512,7 +1519,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" ht="14" customHeight="1">
+    <row r="10" spans="1:31" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>70</v>
       </c>
@@ -1523,7 +1530,7 @@
         <v>0.31</v>
       </c>
       <c r="D10" s="3">
-        <v>0.57</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>32</v>
@@ -1550,28 +1557,28 @@
         <v>-27.8</v>
       </c>
       <c r="M10" s="3">
-        <v>-0.8915981192838</v>
+        <v>-0.89159811928379995</v>
       </c>
       <c r="N10" s="3">
-        <v>0.45149986589819</v>
+        <v>0.45149986589819002</v>
       </c>
       <c r="O10" s="11">
-        <v>-257.98579145029</v>
+        <v>-257.98579145028998</v>
       </c>
       <c r="P10" s="3">
-        <v>97.745845962613</v>
+        <v>97.745845962613004</v>
       </c>
       <c r="Q10" s="11">
-        <v>-449.56412917541</v>
+        <v>-449.56412917541002</v>
       </c>
       <c r="R10" s="3">
-        <v>-66.407453725167</v>
+        <v>-66.407453725167002</v>
       </c>
       <c r="S10" s="11">
         <v>-108</v>
       </c>
       <c r="T10" s="3">
-        <v>40.9191192453572</v>
+        <v>40.919119245357201</v>
       </c>
       <c r="U10" s="11">
         <v>-188.2</v>
@@ -1607,7 +1614,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="11" ht="14" customHeight="1">
+    <row r="11" spans="1:31" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>73</v>
       </c>
@@ -1627,7 +1634,7 @@
         <v>-77.02</v>
       </c>
       <c r="G11" s="11">
-        <v>-135.3</v>
+        <v>-135.30000000000001</v>
       </c>
       <c r="H11" s="3">
         <v>-18.73</v>
@@ -1639,7 +1646,7 @@
         <v>-77.02</v>
       </c>
       <c r="K11" s="11">
-        <v>-135.3</v>
+        <v>-135.30000000000001</v>
       </c>
       <c r="L11" s="3">
         <v>-18.73</v>
@@ -1648,16 +1655,16 @@
         <v>-1.8325814637483</v>
       </c>
       <c r="N11" s="3">
-        <v>0.76080582903376</v>
+        <v>0.76080582903376004</v>
       </c>
       <c r="O11" s="11">
         <v>-197.16063824333</v>
       </c>
       <c r="P11" s="3">
-        <v>76.1246678774466</v>
+        <v>76.124667877446598</v>
       </c>
       <c r="Q11" s="11">
-        <v>-346.34944630385</v>
+        <v>-346.34944630385002</v>
       </c>
       <c r="R11" s="3">
         <v>-47.94623155411</v>
@@ -1669,10 +1676,10 @@
         <v>12.9149586815857</v>
       </c>
       <c r="U11" s="3">
-        <v>-58.76004340151</v>
+        <v>-58.760043401510003</v>
       </c>
       <c r="V11" s="3">
-        <v>-8.1343356460479</v>
+        <v>-8.1343356460478997</v>
       </c>
       <c r="W11" s="2" t="s">
         <v>75</v>
@@ -1702,7 +1709,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" ht="14" customHeight="1">
+    <row r="12" spans="1:31" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>73</v>
       </c>
@@ -1722,7 +1729,7 @@
         <v>-77.02</v>
       </c>
       <c r="G12" s="11">
-        <v>-135.3</v>
+        <v>-135.30000000000001</v>
       </c>
       <c r="H12" s="3">
         <v>-18.73</v>
@@ -1734,7 +1741,7 @@
         <v>-77.02</v>
       </c>
       <c r="K12" s="11">
-        <v>-135.3</v>
+        <v>-135.30000000000001</v>
       </c>
       <c r="L12" s="3">
         <v>-18.73</v>
@@ -1743,31 +1750,31 @@
         <v>-1.8325814637483</v>
       </c>
       <c r="N12" s="3">
-        <v>0.76080582903376</v>
+        <v>0.76080582903376004</v>
       </c>
       <c r="O12" s="11">
-        <v>-654.95346338643</v>
+        <v>-654.95346338643003</v>
       </c>
       <c r="P12" s="3">
-        <v>252.880672936057</v>
+        <v>252.88067293605701</v>
       </c>
       <c r="Q12" s="9">
         <v>-1150.5479563254</v>
       </c>
       <c r="R12" s="11">
-        <v>-159.27393364357</v>
+        <v>-159.27393364356999</v>
       </c>
       <c r="S12" s="11">
         <v>-111.11637204927</v>
       </c>
       <c r="T12" s="3">
-        <v>42.9025640886694</v>
+        <v>42.902564088669401</v>
       </c>
       <c r="U12" s="11">
-        <v>-195.19663903228</v>
+        <v>-195.19663903227999</v>
       </c>
       <c r="V12" s="3">
-        <v>-27.02167811585</v>
+        <v>-27.021678115850001</v>
       </c>
       <c r="W12" s="2" t="s">
         <v>75</v>
@@ -1797,7 +1804,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="13" ht="14" customHeight="1">
+    <row r="13" spans="1:31" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>73</v>
       </c>
@@ -1817,7 +1824,7 @@
         <v>-77.02</v>
       </c>
       <c r="G13" s="11">
-        <v>-135.3</v>
+        <v>-135.30000000000001</v>
       </c>
       <c r="H13" s="3">
         <v>-18.73</v>
@@ -1829,7 +1836,7 @@
         <v>-77.02</v>
       </c>
       <c r="K13" s="11">
-        <v>-135.3</v>
+        <v>-135.30000000000001</v>
       </c>
       <c r="L13" s="3">
         <v>-18.73</v>
@@ -1838,16 +1845,16 @@
         <v>-1.8325814637483</v>
       </c>
       <c r="N13" s="3">
-        <v>0.76080582903376</v>
+        <v>0.76080582903376004</v>
       </c>
       <c r="O13" s="11">
-        <v>-453.97914654428</v>
+        <v>-453.97914654428001</v>
       </c>
       <c r="P13" s="3">
         <v>175.283525463731</v>
       </c>
       <c r="Q13" s="11">
-        <v>-797.49907202598</v>
+        <v>-797.49907202598001</v>
       </c>
       <c r="R13" s="11">
         <v>-110.40027804173</v>
@@ -1856,10 +1863,10 @@
         <v>-77.02</v>
       </c>
       <c r="T13" s="3">
-        <v>29.7377913368535</v>
+        <v>29.737791336853501</v>
       </c>
       <c r="U13" s="11">
-        <v>-135.3</v>
+        <v>-135.30000000000001</v>
       </c>
       <c r="V13" s="3">
         <v>-18.73</v>
@@ -1892,12 +1899,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" ht="14" customHeight="1">
+    <row r="14" spans="1:31" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B14" s="3">
-        <v>0.652</v>
+        <v>0.65200000000000002</v>
       </c>
       <c r="C14" s="3">
         <v>1.028</v>
@@ -1921,43 +1928,43 @@
         <v>78</v>
       </c>
       <c r="J14" s="3">
-        <v>-43.453307392996</v>
+        <v>-43.453307392996003</v>
       </c>
       <c r="K14" s="3">
-        <v>-89.533073929961</v>
+        <v>-89.533073929961006</v>
       </c>
       <c r="L14" s="3">
-        <v>2.61673151750973</v>
+        <v>2.6167315175097299</v>
       </c>
       <c r="M14" s="3">
-        <v>-0.4277107170555</v>
+        <v>-0.42771071705550001</v>
       </c>
       <c r="N14" s="3">
-        <v>0.514</v>
+        <v>0.51400000000000001</v>
       </c>
       <c r="O14" s="3">
-        <v>-64.874082195913</v>
+        <v>-64.874082195913005</v>
       </c>
       <c r="P14" s="3">
-        <v>35.0965740481175</v>
+        <v>35.096574048117503</v>
       </c>
       <c r="Q14" s="11">
         <v>-133.66936479319</v>
       </c>
       <c r="R14" s="3">
-        <v>3.90667743691531</v>
+        <v>3.9066774369153099</v>
       </c>
       <c r="S14" s="3">
-        <v>-43.453307392996</v>
+        <v>-43.453307392996003</v>
       </c>
       <c r="T14" s="3">
-        <v>23.5080353961442</v>
+        <v>23.508035396144201</v>
       </c>
       <c r="U14" s="3">
-        <v>-89.533073929961</v>
+        <v>-89.533073929961006</v>
       </c>
       <c r="V14" s="3">
-        <v>2.61673151750973</v>
+        <v>2.6167315175097299</v>
       </c>
       <c r="W14" s="2" t="s">
         <v>79</v>
@@ -1987,7 +1994,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" ht="14" customHeight="1">
+    <row r="15" spans="1:31" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>80</v>
       </c>
@@ -2004,10 +2011,10 @@
         <v>32</v>
       </c>
       <c r="F15" s="3">
-        <v>-36.3</v>
+        <v>-36.299999999999997</v>
       </c>
       <c r="G15" s="3">
-        <v>-70.6</v>
+        <v>-70.599999999999994</v>
       </c>
       <c r="H15" s="3">
         <v>-2</v>
@@ -2016,16 +2023,16 @@
         <v>46</v>
       </c>
       <c r="J15" s="3">
-        <v>-36.3</v>
+        <v>-36.299999999999997</v>
       </c>
       <c r="K15" s="3">
-        <v>-70.6</v>
+        <v>-70.599999999999994</v>
       </c>
       <c r="L15" s="3">
         <v>-2</v>
       </c>
       <c r="M15" s="3">
-        <v>-0.6931471805599</v>
+        <v>-0.69314718055989999</v>
       </c>
       <c r="N15" s="3">
         <v>0.30057173449127</v>
@@ -2037,22 +2044,22 @@
         <v>50.0300763367526</v>
       </c>
       <c r="Q15" s="11">
-        <v>-201.83191347306</v>
+        <v>-201.83191347306001</v>
       </c>
       <c r="R15" s="3">
         <v>-5.7176179454125</v>
       </c>
       <c r="S15" s="3">
-        <v>-52.36982998427</v>
+        <v>-52.369829984269998</v>
       </c>
       <c r="T15" s="3">
-        <v>25.2476271466307</v>
+        <v>25.247627146630698</v>
       </c>
       <c r="U15" s="11">
-        <v>-101.85426988676</v>
+        <v>-101.85426988675999</v>
       </c>
       <c r="V15" s="3">
-        <v>-2.8853900817779</v>
+        <v>-2.8853900817779001</v>
       </c>
       <c r="W15" s="2" t="s">
         <v>81</v>
@@ -2082,7 +2089,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" ht="14" customHeight="1">
+    <row r="16" spans="1:31" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>82</v>
       </c>
@@ -2123,25 +2130,25 @@
         <v>-1.3577151541999</v>
       </c>
       <c r="N16" s="3">
-        <v>0.55451302937619</v>
+        <v>0.55451302937618996</v>
       </c>
       <c r="O16" s="3">
-        <v>52.743494418145</v>
+        <v>52.743494418144998</v>
       </c>
       <c r="P16" s="3">
-        <v>350.796815190689</v>
+        <v>350.79681519068902</v>
       </c>
       <c r="Q16" s="11">
-        <v>-636.68932547618</v>
+        <v>-636.68932547617999</v>
       </c>
       <c r="R16" s="3">
-        <v>738.408921854029</v>
+        <v>738.40892185402902</v>
       </c>
       <c r="S16" s="3">
         <v>14</v>
       </c>
       <c r="T16" s="3">
-        <v>93.1139558887494</v>
+        <v>93.113955888749402</v>
       </c>
       <c r="U16" s="11">
         <v>-169</v>
@@ -2162,7 +2169,7 @@
         <v>48</v>
       </c>
       <c r="AA16" s="10">
-        <v>37.7</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="AB16" s="2" t="s">
         <v>63</v>
@@ -2177,7 +2184,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" ht="14" customHeight="1">
+    <row r="17" spans="1:31" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>85</v>
       </c>
@@ -2215,28 +2222,28 @@
         <v>15.8</v>
       </c>
       <c r="M17" s="3">
-        <v>-1.6094379124341</v>
+        <v>-1.6094379124341001</v>
       </c>
       <c r="N17" s="3">
-        <v>0.81440250846518</v>
+        <v>0.81440250846518003</v>
       </c>
       <c r="O17" s="11">
-        <v>-213.22313995593</v>
+        <v>-213.22313995593001</v>
       </c>
       <c r="P17" s="3">
-        <v>146.364572274005</v>
+        <v>146.36457227400501</v>
       </c>
       <c r="Q17" s="11">
-        <v>-499.85863292301</v>
+        <v>-499.85863292301002</v>
       </c>
       <c r="R17" s="3">
-        <v>73.8799476163102</v>
+        <v>73.879947616310204</v>
       </c>
       <c r="S17" s="3">
         <v>-45.6</v>
       </c>
       <c r="T17" s="3">
-        <v>31.3015955823275</v>
+        <v>31.301595582327501</v>
       </c>
       <c r="U17" s="11">
         <v>-106.9</v>
@@ -2272,7 +2279,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" ht="14" customHeight="1">
+    <row r="18" spans="1:31" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>87</v>
       </c>
@@ -2310,34 +2317,34 @@
         <v>311.36</v>
       </c>
       <c r="M18" s="3">
-        <v>-1.6259957752857</v>
+        <v>-1.6259957752856999</v>
       </c>
       <c r="N18" s="3">
-        <v>0.50967940542783</v>
+        <v>0.50967940542782997</v>
       </c>
       <c r="O18" s="3">
         <v>113.26135347042</v>
       </c>
       <c r="P18" s="3">
-        <v>283.765201608405</v>
+        <v>283.76520160840499</v>
       </c>
       <c r="Q18" s="11">
-        <v>-442.91897168644</v>
+        <v>-442.91897168643999</v>
       </c>
       <c r="R18" s="3">
-        <v>669.420178750004</v>
+        <v>669.42017875000397</v>
       </c>
       <c r="S18" s="3">
-        <v>22.8786333066634</v>
+        <v>22.878633306663399</v>
       </c>
       <c r="T18" s="3">
-        <v>57.3201696241911</v>
+        <v>57.320169624191102</v>
       </c>
       <c r="U18" s="3">
-        <v>-89.469006216887</v>
+        <v>-89.469006216886996</v>
       </c>
       <c r="V18" s="3">
-        <v>135.221929885395</v>
+        <v>135.22192988539501</v>
       </c>
       <c r="W18" s="2" t="s">
         <v>88</v>
@@ -2352,7 +2359,7 @@
         <v>48</v>
       </c>
       <c r="AA18" s="12">
-        <v>39.3571428571429</v>
+        <v>39.357142857142897</v>
       </c>
       <c r="AB18" s="2" t="s">
         <v>68</v>
@@ -2367,15 +2374,15 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" ht="14" customHeight="1">
+    <row r="19" spans="1:31" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B19" s="3">
-        <v>0.279</v>
+        <v>0.27900000000000003</v>
       </c>
       <c r="C19" s="3">
-        <v>0.138</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>44</v>
@@ -2405,16 +2412,16 @@
         <v>191.2</v>
       </c>
       <c r="M19" s="3">
-        <v>-1.3859717089067</v>
+        <v>-1.3859717089067001</v>
       </c>
       <c r="N19" s="3">
-        <v>0.46782093101095</v>
+        <v>0.46782093101095001</v>
       </c>
       <c r="O19" s="11">
-        <v>-521.69799685074</v>
+        <v>-521.69799685073997</v>
       </c>
       <c r="P19" s="3">
-        <v>431.888327953627</v>
+        <v>431.88832795362703</v>
       </c>
       <c r="Q19" s="9">
         <v>-1368.2684767664</v>
@@ -2423,16 +2430,16 @@
         <v>324.70265949825</v>
       </c>
       <c r="S19" s="11">
-        <v>-133.41526484068</v>
+        <v>-133.41526484068001</v>
       </c>
       <c r="T19" s="3">
         <v>110.44799098973</v>
       </c>
       <c r="U19" s="11">
-        <v>-349.91106406945</v>
+        <v>-349.91106406944999</v>
       </c>
       <c r="V19" s="3">
-        <v>83.0371049399019</v>
+        <v>83.037104939901894</v>
       </c>
       <c r="W19" s="2" t="s">
         <v>90</v>
@@ -2462,15 +2469,15 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" ht="14" customHeight="1">
+    <row r="20" spans="1:31" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>91</v>
       </c>
       <c r="B20" s="3">
-        <v>1.15</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="C20" s="3">
-        <v>0.848</v>
+        <v>0.84799999999999998</v>
       </c>
       <c r="D20" s="3">
         <v>1.59</v>
@@ -2479,7 +2486,7 @@
         <v>32</v>
       </c>
       <c r="F20" s="3">
-        <v>-39.3</v>
+        <v>-39.299999999999997</v>
       </c>
       <c r="G20" s="11">
         <v>-111</v>
@@ -2491,7 +2498,7 @@
         <v>58</v>
       </c>
       <c r="J20" s="3">
-        <v>-39.3</v>
+        <v>-39.299999999999997</v>
       </c>
       <c r="K20" s="11">
         <v>-111</v>
@@ -2500,28 +2507,28 @@
         <v>31.8</v>
       </c>
       <c r="M20" s="3">
-        <v>0.13976194237516</v>
+        <v>0.13976194237515999</v>
       </c>
       <c r="N20" s="3">
-        <v>0.46598829665119</v>
+        <v>0.46598829665119001</v>
       </c>
       <c r="O20" s="3">
-        <v>-33.424428028442</v>
+        <v>-33.424428028442001</v>
       </c>
       <c r="P20" s="3">
-        <v>30.9828635640361</v>
+        <v>30.982863564036101</v>
       </c>
       <c r="Q20" s="3">
-        <v>-94.404873057432</v>
+        <v>-94.404873057431999</v>
       </c>
       <c r="R20" s="3">
         <v>27.0457203894264</v>
       </c>
       <c r="S20" s="3">
-        <v>-39.3</v>
+        <v>-39.299999999999997</v>
       </c>
       <c r="T20" s="3">
-        <v>36.4292408244203</v>
+        <v>36.429240824420297</v>
       </c>
       <c r="U20" s="11">
         <v>-111</v>
@@ -2557,7 +2564,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" ht="14" customHeight="1">
+    <row r="21" spans="1:31" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>93</v>
       </c>
@@ -2595,31 +2602,31 @@
         <v>-27.1</v>
       </c>
       <c r="M21" s="3">
-        <v>0.18232155679395</v>
+        <v>0.18232155679395001</v>
       </c>
       <c r="N21" s="3">
-        <v>0.42651807896529</v>
+        <v>0.42651807896528998</v>
       </c>
       <c r="O21" s="3">
-        <v>-34.174551399754</v>
+        <v>-34.174551399754002</v>
       </c>
       <c r="P21" s="3">
-        <v>12.5244224136026</v>
+        <v>12.524422413602601</v>
       </c>
       <c r="Q21" s="3">
-        <v>-58.721968257581</v>
+        <v>-58.721968257580997</v>
       </c>
       <c r="R21" s="3">
         <v>-9.6271345419265</v>
       </c>
       <c r="S21" s="3">
-        <v>-41.779129159093</v>
+        <v>-41.779129159093003</v>
       </c>
       <c r="T21" s="3">
         <v>15.3113776254195</v>
       </c>
       <c r="U21" s="3">
-        <v>-71.788877858608</v>
+        <v>-71.788877858608004</v>
       </c>
       <c r="V21" s="3">
         <v>-11.769380459578</v>
@@ -2652,7 +2659,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" ht="14" customHeight="1">
+    <row r="22" spans="1:31" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>95</v>
       </c>
@@ -2690,13 +2697,13 @@
         <v>-4</v>
       </c>
       <c r="M22" s="3">
-        <v>-0.634878272436</v>
+        <v>-0.63487827243600004</v>
       </c>
       <c r="N22" s="3">
-        <v>0.46472003097063</v>
+        <v>0.46472003097063003</v>
       </c>
       <c r="O22" s="3">
-        <v>-84.899143893611</v>
+        <v>-84.899143893610997</v>
       </c>
       <c r="P22" s="3">
         <v>40.020850914693</v>
@@ -2705,7 +2712,7 @@
         <v>-164.26138709851</v>
       </c>
       <c r="R22" s="3">
-        <v>-7.3825342516184</v>
+        <v>-7.3825342516183996</v>
       </c>
       <c r="S22" s="3">
         <v>-46</v>
@@ -2720,7 +2727,7 @@
         <v>-4</v>
       </c>
       <c r="W22" s="2" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="X22" s="6">
         <v>1533</v>
@@ -2747,9 +2754,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" ht="14" customHeight="1">
+    <row r="23" spans="1:31" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B23" s="3">
         <v>2.33</v>
@@ -2785,28 +2792,28 @@
         <v>61</v>
       </c>
       <c r="M23" s="3">
-        <v>0.84586826757761</v>
+        <v>0.84586826757761002</v>
       </c>
       <c r="N23" s="3">
-        <v>0.5431707204154</v>
+        <v>0.54317072041540004</v>
       </c>
       <c r="O23" s="3">
-        <v>-19.699032131503</v>
+        <v>-19.699032131502999</v>
       </c>
       <c r="P23" s="3">
-        <v>23.0125165291343</v>
+        <v>23.012516529134299</v>
       </c>
       <c r="Q23" s="3">
-        <v>-64.802735722239</v>
+        <v>-64.802735722239007</v>
       </c>
       <c r="R23" s="3">
-        <v>25.4046714592326</v>
+        <v>25.404671459232599</v>
       </c>
       <c r="S23" s="3">
         <v>-47.3</v>
       </c>
       <c r="T23" s="3">
-        <v>55.25611738494</v>
+        <v>55.256117384939998</v>
       </c>
       <c r="U23" s="11">
         <v>-155.6</v>
@@ -2815,7 +2822,7 @@
         <v>61</v>
       </c>
       <c r="W23" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="X23" s="6">
         <v>214</v>
@@ -2842,9 +2849,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" ht="14" customHeight="1">
+    <row r="24" spans="1:31" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B24" s="3">
         <v>0.7</v>
@@ -2880,28 +2887,28 @@
         <v>69</v>
       </c>
       <c r="M24" s="3">
-        <v>-0.3566749439387</v>
+        <v>-0.35667494393869997</v>
       </c>
       <c r="N24" s="3">
         <v>0.43572690682262</v>
       </c>
       <c r="O24" s="3">
-        <v>-50.440376773772</v>
+        <v>-50.440376773772002</v>
       </c>
       <c r="P24" s="3">
-        <v>74.7040282150914</v>
+        <v>74.704028215091398</v>
       </c>
       <c r="Q24" s="11">
         <v>-196.15702078689</v>
       </c>
       <c r="R24" s="3">
-        <v>96.6773888163961</v>
+        <v>96.677388816396103</v>
       </c>
       <c r="S24" s="3">
         <v>-36</v>
       </c>
       <c r="T24" s="3">
-        <v>53.3173062486263</v>
+        <v>53.317306248626302</v>
       </c>
       <c r="U24" s="11">
         <v>-140</v>
@@ -2910,7 +2917,7 @@
         <v>69</v>
       </c>
       <c r="W24" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="X24" s="6">
         <v>338</v>
@@ -2937,9 +2944,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" ht="14" customHeight="1">
+    <row r="25" spans="1:31" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B25" s="3">
         <v>0.7</v>
@@ -2975,16 +2982,16 @@
         <v>232</v>
       </c>
       <c r="M25" s="3">
-        <v>-0.3566749439387</v>
+        <v>-0.35667494393869997</v>
       </c>
       <c r="N25" s="3">
         <v>0.43572690682262</v>
       </c>
       <c r="O25" s="3">
-        <v>154.123373475414</v>
+        <v>154.12337347541401</v>
       </c>
       <c r="P25" s="3">
-        <v>87.5717077162556</v>
+        <v>87.571707716255602</v>
       </c>
       <c r="Q25" s="3">
         <v>-18.21458050164</v>
@@ -2996,7 +3003,7 @@
         <v>110</v>
       </c>
       <c r="T25" s="3">
-        <v>62.5011484732701</v>
+        <v>62.501148473270099</v>
       </c>
       <c r="U25" s="3">
         <v>-13</v>
@@ -3005,7 +3012,7 @@
         <v>232</v>
       </c>
       <c r="W25" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="X25" s="6">
         <v>298</v>
@@ -3032,27 +3039,27 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" ht="14" customHeight="1">
+    <row r="26" spans="1:31" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B26" s="3">
-        <v>1.566</v>
+        <v>1.5660000000000001</v>
       </c>
       <c r="C26" s="3">
-        <v>0.3187</v>
+        <v>0.31869999999999998</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>44</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F26" s="3">
         <v>62.66</v>
       </c>
       <c r="G26" s="3">
-        <v>-32.05</v>
+        <v>-32.049999999999997</v>
       </c>
       <c r="H26" s="3">
         <v>157.38</v>
@@ -3064,43 +3071,43 @@
         <v>62.66</v>
       </c>
       <c r="K26" s="3">
-        <v>-32.05</v>
+        <v>-32.049999999999997</v>
       </c>
       <c r="L26" s="3">
         <v>157.38</v>
       </c>
       <c r="M26" s="3">
-        <v>0.44852459756861</v>
+        <v>0.44852459756861002</v>
       </c>
       <c r="N26" s="3">
-        <v>0.3187</v>
+        <v>0.31869999999999998</v>
       </c>
       <c r="O26" s="3">
-        <v>39.5987089026308</v>
+        <v>39.598708902630797</v>
       </c>
       <c r="P26" s="3">
         <v>30.5394568108252</v>
       </c>
       <c r="Q26" s="3">
-        <v>-20.254366746398</v>
+        <v>-20.254366746397999</v>
       </c>
       <c r="R26" s="3">
-        <v>99.4581041668695</v>
+        <v>99.458104166869504</v>
       </c>
       <c r="S26" s="3">
         <v>62.66</v>
       </c>
       <c r="T26" s="3">
-        <v>48.3248675726186</v>
+        <v>48.324867572618601</v>
       </c>
       <c r="U26" s="3">
-        <v>-32.05</v>
+        <v>-32.049999999999997</v>
       </c>
       <c r="V26" s="3">
         <v>157.38</v>
       </c>
       <c r="W26" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="X26" s="6">
         <v>113</v>
@@ -3127,21 +3134,21 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" ht="14" customHeight="1">
+    <row r="27" spans="1:31" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B27" s="3">
-        <v>1.211</v>
+        <v>1.2110000000000001</v>
       </c>
       <c r="C27" s="3">
-        <v>0.3139</v>
+        <v>0.31390000000000001</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>44</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F27" s="3">
         <v>-10.08</v>
@@ -3165,19 +3172,19 @@
         <v>91.29</v>
       </c>
       <c r="M27" s="3">
-        <v>0.19144646457096</v>
+        <v>0.19144646457096001</v>
       </c>
       <c r="N27" s="3">
-        <v>0.3139</v>
+        <v>0.31390000000000001</v>
       </c>
       <c r="O27" s="3">
-        <v>-8.2401194978635</v>
+        <v>-8.2401194978634997</v>
       </c>
       <c r="P27" s="3">
         <v>42.2820225940103</v>
       </c>
       <c r="Q27" s="3">
-        <v>-91.115448336495</v>
+        <v>-91.115448336495007</v>
       </c>
       <c r="R27" s="3">
         <v>74.6270346190433</v>
@@ -3186,7 +3193,7 @@
         <v>-10.08</v>
       </c>
       <c r="T27" s="3">
-        <v>51.7228891957368</v>
+        <v>51.722889195736798</v>
       </c>
       <c r="U27" s="11">
         <v>-111.46</v>
@@ -3195,7 +3202,7 @@
         <v>91.29</v>
       </c>
       <c r="W27" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="X27" s="6">
         <v>117</v>
@@ -3222,9 +3229,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" ht="14" customHeight="1">
+    <row r="28" spans="1:31" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B28" s="3">
         <v>1.55</v>
@@ -3260,16 +3267,16 @@
         <v>110</v>
       </c>
       <c r="M28" s="3">
-        <v>0.43825493093116</v>
+        <v>0.43825493093116002</v>
       </c>
       <c r="N28" s="3">
         <v>0.77013257352427</v>
       </c>
       <c r="O28" s="3">
-        <v>12.1515546334008</v>
+        <v>12.151554633400799</v>
       </c>
       <c r="P28" s="3">
-        <v>26.3495184601939</v>
+        <v>26.349518460193899</v>
       </c>
       <c r="Q28" s="3">
         <v>-36.454663900202</v>
@@ -3290,7 +3297,7 @@
         <v>110</v>
       </c>
       <c r="W28" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="X28" s="6">
         <v>117</v>
@@ -3317,9 +3324,9 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" ht="14" customHeight="1">
+    <row r="29" spans="1:31" ht="13.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B29" s="3">
         <v>1.58</v>
@@ -3355,22 +3362,22 @@
         <v>-0.01</v>
       </c>
       <c r="M29" s="3">
-        <v>0.45742484703888</v>
+        <v>0.45742484703887998</v>
       </c>
       <c r="N29" s="3">
-        <v>0.78438621736904</v>
+        <v>0.78438621736904002</v>
       </c>
       <c r="O29" s="3">
-        <v>-47.578087911863</v>
+        <v>-47.578087911863001</v>
       </c>
       <c r="P29" s="3">
-        <v>24.2734635210824</v>
+        <v>24.273463521082402</v>
       </c>
       <c r="Q29" s="3">
-        <v>-95.156175823726</v>
+        <v>-95.156175823726002</v>
       </c>
       <c r="R29" s="3">
-        <v>-0.005947260989</v>
+        <v>-5.9472609890000002E-3</v>
       </c>
       <c r="S29" s="3">
         <v>-80</v>
@@ -3385,7 +3392,7 @@
         <v>-0.01</v>
       </c>
       <c r="W29" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X29" s="6">
         <v>106</v>
@@ -3412,14 +3419,11 @@
         <v>56</v>
       </c>
     </row>
-    <row r="30" ht="12" customHeight="1"/>
   </sheetData>
-  <printOptions headings="0" horizontalCentered="0" verticalCentered="0" gridLines="0"/>
   <pageMargins left="0.05" right="0.05" top="0.5" bottom="0.5" header="0" footer="0"/>
-  <pageSetup paperSize="1" fitToWidth="1" fitToHeight="1" scale="100" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>The SAS System</oddHeader>
-    <oddFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>